<commit_message>
Spa Update & schedule via excel sheet
</commit_message>
<xml_diff>
--- a/F124_season.xlsx
+++ b/F124_season.xlsx
@@ -6,6 +6,7 @@
     <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="PythonReadyData" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Schedule" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="68">
   <si>
     <t>Suzuka</t>
   </si>
@@ -152,12 +153,78 @@
   <si>
     <t>Starting</t>
   </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Pre-Season: Miami</t>
+  </si>
+  <si>
+    <t>11/13/2024</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>11/20/2024</t>
+  </si>
+  <si>
+    <t>12/4/2024</t>
+  </si>
+  <si>
+    <t>12/11/2024</t>
+  </si>
+  <si>
+    <t>1/1/2025</t>
+  </si>
+  <si>
+    <t>Tentative</t>
+  </si>
+  <si>
+    <t>1/2/2025</t>
+  </si>
+  <si>
+    <t>China &amp; Sprint</t>
+  </si>
+  <si>
+    <t>1/8/2025</t>
+  </si>
+  <si>
+    <t>1/15/2025</t>
+  </si>
+  <si>
+    <t>1/22/2025</t>
+  </si>
+  <si>
+    <t>1/23/2025</t>
+  </si>
+  <si>
+    <t>1/29/2025</t>
+  </si>
+  <si>
+    <t>Austria &amp; Sprint</t>
+  </si>
+  <si>
+    <t>2/5/2025</t>
+  </si>
+  <si>
+    <t>COTA &amp; Sprint</t>
+  </si>
+  <si>
+    <t>2/12/2025</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -173,6 +240,11 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12.0"/>
+      <color rgb="FF31333F"/>
+      <name val="&quot;Source Sans Pro&quot;"/>
     </font>
   </fonts>
   <fills count="5">
@@ -418,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -485,6 +557,12 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -502,6 +580,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -6913,4 +6995,177 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="16.5"/>
+    <col customWidth="1" min="2" max="2" width="25.38"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated race schedule excel sheet
</commit_message>
<xml_diff>
--- a/F124_season.xlsx
+++ b/F124_season.xlsx
@@ -184,16 +184,16 @@
     <t>1/1/2025</t>
   </si>
   <si>
-    <t>Tentative</t>
-  </si>
-  <si>
-    <t>1/2/2025</t>
+    <t>Upcoming</t>
   </si>
   <si>
     <t>China &amp; Sprint</t>
   </si>
   <si>
     <t>1/8/2025</t>
+  </si>
+  <si>
+    <t>Tentative</t>
   </si>
   <si>
     <t>1/15/2025</t>
@@ -7082,7 +7082,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>56</v>
@@ -7090,13 +7090,13 @@
     </row>
     <row r="8">
       <c r="A8" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="C8" s="32" t="s">
         <v>59</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9">
@@ -7107,7 +7107,7 @@
         <v>60</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10">
@@ -7118,7 +7118,7 @@
         <v>61</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
@@ -7129,7 +7129,7 @@
         <v>62</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12">
@@ -7140,7 +7140,7 @@
         <v>63</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
@@ -7151,7 +7151,7 @@
         <v>65</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
@@ -7162,7 +7162,7 @@
         <v>67</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>